<commit_message>
feat(model): add predictor and demo
</commit_message>
<xml_diff>
--- a/model/model-senior/predict/predict_data.xlsx
+++ b/model/model-senior/predict/predict_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LiqisPode\school\BlueSpace\test\predict\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LiqisPode\school\BlueSpace\test\model-senior\predict\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA56F0C-9A69-4A18-B37C-ABEBDDFC44A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AFCECB-C871-482F-9272-C30124DCDD38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19680" yWindow="0" windowWidth="18720" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="388">
-  <si>
-    <t>Radial Velocity</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="357">
   <si>
     <t>rowid</t>
   </si>
@@ -1098,97 +1095,8 @@
     <t>st_colorn</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>Msini</t>
-  </si>
-  <si>
-    <t>V (Johnson)</t>
-  </si>
-  <si>
-    <t>Ground</t>
-  </si>
-  <si>
-    <t>[Fe/H]</t>
-  </si>
-  <si>
-    <t>W. M. Keck Observatory</t>
-  </si>
-  <si>
-    <t>Imaging</t>
-  </si>
-  <si>
-    <t>Mass</t>
-  </si>
-  <si>
-    <t>24 Sex</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>24 Sex c</t>
-  </si>
-  <si>
-    <t>10h23m28.37s</t>
-  </si>
-  <si>
-    <t>-00d54m08.1s</t>
-  </si>
-  <si>
-    <t>&lt;a refstr=JOHNSON_ET_AL__2010 href=http://adsabs.harvard.edu/cgi-bin/nph-bib_query?bibcode=2010arXiv1007.4552J target=ref&gt; Johnson et al. 2010 &lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Lick Observatory</t>
-  </si>
-  <si>
-    <t>3.0 m C. Donald Shane Telescope</t>
-  </si>
-  <si>
-    <t>Hamilton Echelle Spectrograph</t>
-  </si>
-  <si>
-    <t>http://exoplanet.eu/catalog/24_sex_c/</t>
-  </si>
-  <si>
-    <t>http://exoplanets.org/detail/24_Sex_c</t>
-  </si>
-  <si>
-    <t>HD 90043</t>
-  </si>
-  <si>
-    <t>HIP 50887</t>
-  </si>
-  <si>
-    <t>K0 IV</t>
-  </si>
-  <si>
-    <t>2MASS J01225093-2439505</t>
-  </si>
-  <si>
-    <t>2MASS J01225093-2439505 b</t>
-  </si>
-  <si>
-    <t>01h22m50.94s</t>
-  </si>
-  <si>
-    <t>-24d39m50.6s</t>
-  </si>
-  <si>
-    <t>&lt;a refstr=BOWLER_ET_AL__2013 href=http://adsabs.harvard.edu/abs/2013ApJ...774...55B target=ref&gt; Bowler et al. 2013 &lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>10 m Keck II Telescope</t>
-  </si>
-  <si>
-    <t>NIRC2 Camera</t>
-  </si>
-  <si>
-    <t>http://exoplanet.eu/catalog/2m_0122-24_b/</t>
-  </si>
-  <si>
-    <t>M3.5 V</t>
+    <t>liqi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1528,2275 +1436,1105 @@
   <dimension ref="A1:MR10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:356" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="CM1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CM1" s="1" t="s">
+      <c r="CN1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="CO1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="CP1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CR1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="CS1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="CT1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="CU1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="CV1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="CY1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DG1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="DG1" s="1" t="s">
+      <c r="DH1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="DH1" s="1" t="s">
+      <c r="DI1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="DK1" s="1" t="s">
+      <c r="DL1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="DL1" s="1" t="s">
+      <c r="DM1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="DM1" s="1" t="s">
+      <c r="DN1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="DN1" s="1" t="s">
+      <c r="DO1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="DO1" s="1" t="s">
+      <c r="DP1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="DP1" s="1" t="s">
+      <c r="DQ1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="DQ1" s="1" t="s">
+      <c r="DR1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="DR1" s="1" t="s">
+      <c r="DS1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="DS1" s="1" t="s">
+      <c r="DT1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="DT1" s="1" t="s">
+      <c r="DU1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="DU1" s="1" t="s">
+      <c r="DV1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="DV1" s="1" t="s">
+      <c r="DW1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="DW1" s="1" t="s">
+      <c r="DX1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="DX1" s="1" t="s">
+      <c r="DY1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="DY1" s="1" t="s">
+      <c r="DZ1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="DZ1" s="1" t="s">
+      <c r="EA1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="EA1" s="1" t="s">
+      <c r="EB1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="EB1" s="1" t="s">
+      <c r="EC1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="EC1" s="1" t="s">
+      <c r="ED1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="ED1" s="1" t="s">
+      <c r="EE1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="EE1" s="1" t="s">
+      <c r="EF1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="EF1" s="1" t="s">
+      <c r="EG1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="EG1" s="1" t="s">
+      <c r="EH1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="EH1" s="1" t="s">
+      <c r="EI1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="EI1" s="1" t="s">
+      <c r="EJ1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="EJ1" s="1" t="s">
+      <c r="EK1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="EK1" s="1" t="s">
+      <c r="EL1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="EL1" s="1" t="s">
+      <c r="EM1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="EM1" s="1" t="s">
+      <c r="EN1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="EN1" s="1" t="s">
+      <c r="EO1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="EO1" s="1" t="s">
+      <c r="EP1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="EP1" s="1" t="s">
+      <c r="EQ1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="EQ1" s="1" t="s">
+      <c r="ER1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="ER1" s="1" t="s">
+      <c r="ES1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="ES1" s="1" t="s">
+      <c r="ET1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="ET1" s="1" t="s">
+      <c r="EU1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="EU1" s="1" t="s">
+      <c r="EV1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="EV1" s="1" t="s">
+      <c r="EW1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="EW1" s="1" t="s">
+      <c r="EX1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="EX1" s="1" t="s">
+      <c r="EY1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="EY1" s="1" t="s">
+      <c r="EZ1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="EZ1" s="1" t="s">
+      <c r="FA1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="FA1" s="1" t="s">
+      <c r="FB1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="FB1" s="1" t="s">
+      <c r="FC1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="FC1" s="1" t="s">
+      <c r="FD1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="FD1" s="1" t="s">
+      <c r="FE1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="FE1" s="1" t="s">
+      <c r="FF1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="FF1" s="1" t="s">
+      <c r="FG1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="FG1" s="1" t="s">
+      <c r="FH1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="FH1" s="1" t="s">
+      <c r="FI1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="FI1" s="1" t="s">
+      <c r="FJ1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="FJ1" s="1" t="s">
+      <c r="FK1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="FK1" s="1" t="s">
+      <c r="FL1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="FL1" s="1" t="s">
+      <c r="FM1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="FM1" s="1" t="s">
+      <c r="FN1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="FN1" s="1" t="s">
+      <c r="FO1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="FO1" s="1" t="s">
+      <c r="FP1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="FP1" s="1" t="s">
+      <c r="FQ1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="FQ1" s="1" t="s">
+      <c r="FR1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="FR1" s="1" t="s">
+      <c r="FS1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="FS1" s="1" t="s">
+      <c r="FT1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="FT1" s="1" t="s">
+      <c r="FU1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="FU1" s="1" t="s">
+      <c r="FV1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="FV1" s="1" t="s">
+      <c r="FW1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="FW1" s="1" t="s">
+      <c r="FX1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="FX1" s="1" t="s">
+      <c r="FY1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="FY1" s="1" t="s">
+      <c r="FZ1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="FZ1" s="1" t="s">
+      <c r="GA1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="GA1" s="1" t="s">
+      <c r="GB1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="GB1" s="1" t="s">
+      <c r="GC1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="GC1" s="1" t="s">
+      <c r="GD1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="GD1" s="1" t="s">
+      <c r="GE1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="GE1" s="1" t="s">
+      <c r="GF1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="GF1" s="1" t="s">
+      <c r="GG1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="GG1" s="1" t="s">
+      <c r="GH1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="GH1" s="1" t="s">
+      <c r="GI1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="GI1" s="1" t="s">
+      <c r="GJ1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="GJ1" s="1" t="s">
+      <c r="GK1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="GK1" s="1" t="s">
+      <c r="GL1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="GL1" s="1" t="s">
+      <c r="GM1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="GM1" s="1" t="s">
+      <c r="GN1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="GN1" s="1" t="s">
+      <c r="GO1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="GO1" s="1" t="s">
+      <c r="GP1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="GP1" s="1" t="s">
+      <c r="GQ1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="GQ1" s="1" t="s">
+      <c r="GR1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="GR1" s="1" t="s">
+      <c r="GS1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="GS1" s="1" t="s">
+      <c r="GT1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="GT1" s="1" t="s">
+      <c r="GU1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="GU1" s="1" t="s">
+      <c r="GV1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="GV1" s="1" t="s">
+      <c r="GW1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="GW1" s="1" t="s">
+      <c r="GX1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="GX1" s="1" t="s">
+      <c r="GY1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="GY1" s="1" t="s">
+      <c r="GZ1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="GZ1" s="1" t="s">
+      <c r="HA1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="HA1" s="1" t="s">
+      <c r="HB1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="HB1" s="1" t="s">
+      <c r="HC1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="HC1" s="1" t="s">
+      <c r="HD1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="HD1" s="1" t="s">
+      <c r="HE1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="HE1" s="1" t="s">
+      <c r="HF1" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="HF1" s="1" t="s">
+      <c r="HG1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="HG1" s="1" t="s">
+      <c r="HH1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="HH1" s="1" t="s">
+      <c r="HI1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="HI1" s="1" t="s">
+      <c r="HJ1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="HJ1" s="1" t="s">
+      <c r="HK1" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="HK1" s="1" t="s">
+      <c r="HL1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="HL1" s="1" t="s">
+      <c r="HM1" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="HM1" s="1" t="s">
+      <c r="HN1" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="HN1" s="1" t="s">
+      <c r="HO1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="HO1" s="1" t="s">
+      <c r="HP1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="HP1" s="1" t="s">
+      <c r="HQ1" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="HQ1" s="1" t="s">
+      <c r="HR1" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="HR1" s="1" t="s">
+      <c r="HS1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="HS1" s="1" t="s">
+      <c r="HT1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="HT1" s="1" t="s">
+      <c r="HU1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="HU1" s="1" t="s">
+      <c r="HV1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="HV1" s="1" t="s">
+      <c r="HW1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="HW1" s="1" t="s">
+      <c r="HX1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="HX1" s="1" t="s">
+      <c r="HY1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="HY1" s="1" t="s">
+      <c r="HZ1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="HZ1" s="1" t="s">
+      <c r="IA1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="IA1" s="1" t="s">
+      <c r="IB1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="IB1" s="1" t="s">
+      <c r="IC1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="IC1" s="1" t="s">
+      <c r="ID1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="ID1" s="1" t="s">
+      <c r="IE1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="IE1" s="1" t="s">
+      <c r="IF1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="IF1" s="1" t="s">
+      <c r="IG1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="IG1" s="1" t="s">
+      <c r="IH1" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="IH1" s="1" t="s">
+      <c r="II1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="II1" s="1" t="s">
+      <c r="IJ1" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="IJ1" s="1" t="s">
+      <c r="IK1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="IK1" s="1" t="s">
+      <c r="IL1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="IL1" s="1" t="s">
+      <c r="IM1" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="IM1" s="1" t="s">
+      <c r="IN1" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="IN1" s="1" t="s">
+      <c r="IO1" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="IO1" s="1" t="s">
+      <c r="IP1" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="IP1" s="1" t="s">
+      <c r="IQ1" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="IQ1" s="1" t="s">
+      <c r="IR1" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="IR1" s="1" t="s">
+      <c r="IS1" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="IS1" s="1" t="s">
+      <c r="IT1" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="IT1" s="1" t="s">
+      <c r="IU1" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="IU1" s="1" t="s">
+      <c r="IV1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="IV1" s="1" t="s">
+      <c r="IW1" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="IW1" s="1" t="s">
+      <c r="IX1" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="IX1" s="1" t="s">
+      <c r="IY1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="IY1" s="1" t="s">
+      <c r="IZ1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="IZ1" s="1" t="s">
+      <c r="JA1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="JA1" s="1" t="s">
+      <c r="JB1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="JB1" s="1" t="s">
+      <c r="JC1" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="JC1" s="1" t="s">
+      <c r="JD1" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="JD1" s="1" t="s">
+      <c r="JE1" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="JE1" s="1" t="s">
+      <c r="JF1" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="JF1" s="1" t="s">
+      <c r="JG1" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="JG1" s="1" t="s">
+      <c r="JH1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="JH1" s="1" t="s">
+      <c r="JI1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="JI1" s="1" t="s">
+      <c r="JJ1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="JJ1" s="1" t="s">
+      <c r="JK1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="JK1" s="1" t="s">
+      <c r="JL1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="JL1" s="1" t="s">
+      <c r="JM1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="JM1" s="1" t="s">
+      <c r="JN1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="JN1" s="1" t="s">
+      <c r="JO1" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="JO1" s="1" t="s">
+      <c r="JP1" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="JP1" s="1" t="s">
+      <c r="JQ1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="JQ1" s="1" t="s">
+      <c r="JR1" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="JR1" s="1" t="s">
+      <c r="JS1" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="JS1" s="1" t="s">
+      <c r="JT1" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="JT1" s="1" t="s">
+      <c r="JU1" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="JU1" s="1" t="s">
+      <c r="JV1" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="JV1" s="1" t="s">
+      <c r="JW1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="JW1" s="1" t="s">
+      <c r="JX1" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="JX1" s="1" t="s">
+      <c r="JY1" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="JY1" s="1" t="s">
+      <c r="JZ1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="JZ1" s="1" t="s">
+      <c r="KA1" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="KA1" s="1" t="s">
+      <c r="KB1" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="KB1" s="1" t="s">
+      <c r="KC1" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="KC1" s="1" t="s">
+      <c r="KD1" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="KD1" s="1" t="s">
+      <c r="KE1" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="KE1" s="1" t="s">
+      <c r="KF1" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="KF1" s="1" t="s">
+      <c r="KG1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="KG1" s="1" t="s">
+      <c r="KH1" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="KH1" s="1" t="s">
+      <c r="KI1" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="KI1" s="1" t="s">
+      <c r="KJ1" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="KJ1" s="1" t="s">
+      <c r="KK1" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="KK1" s="1" t="s">
+      <c r="KL1" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="KL1" s="1" t="s">
+      <c r="KM1" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="KM1" s="1" t="s">
+      <c r="KN1" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="KN1" s="1" t="s">
+      <c r="KO1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="KO1" s="1" t="s">
+      <c r="KP1" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="KP1" s="1" t="s">
+      <c r="KQ1" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="KQ1" s="1" t="s">
+      <c r="KR1" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="KR1" s="1" t="s">
+      <c r="KS1" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="KS1" s="1" t="s">
+      <c r="KT1" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="KT1" s="1" t="s">
+      <c r="KU1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="KU1" s="1" t="s">
+      <c r="KV1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="KV1" s="1" t="s">
+      <c r="KW1" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="KW1" s="1" t="s">
+      <c r="KX1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="KX1" s="1" t="s">
+      <c r="KY1" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="KY1" s="1" t="s">
+      <c r="KZ1" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="KZ1" s="1" t="s">
+      <c r="LA1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="LA1" s="1" t="s">
+      <c r="LB1" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="LB1" s="1" t="s">
+      <c r="LC1" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="LC1" s="1" t="s">
+      <c r="LD1" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="LD1" s="1" t="s">
+      <c r="LE1" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="LE1" s="1" t="s">
+      <c r="LF1" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="LF1" s="1" t="s">
+      <c r="LG1" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="LG1" s="1" t="s">
+      <c r="LH1" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="LH1" s="1" t="s">
+      <c r="LI1" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="LI1" s="1" t="s">
+      <c r="LJ1" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="LJ1" s="1" t="s">
+      <c r="LK1" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="LK1" s="1" t="s">
+      <c r="LL1" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="LL1" s="1" t="s">
+      <c r="LM1" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="LM1" s="1" t="s">
+      <c r="LN1" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="LN1" s="1" t="s">
+      <c r="LO1" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="LO1" s="1" t="s">
+      <c r="LP1" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="LP1" s="1" t="s">
+      <c r="LQ1" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="LQ1" s="1" t="s">
+      <c r="LR1" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="LR1" s="1" t="s">
+      <c r="LS1" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="LS1" s="1" t="s">
+      <c r="LT1" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="LT1" s="1" t="s">
+      <c r="LU1" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="LU1" s="1" t="s">
+      <c r="LV1" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="LV1" s="1" t="s">
+      <c r="LW1" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="LW1" s="1" t="s">
+      <c r="LX1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="LX1" s="1" t="s">
+      <c r="LY1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="LY1" s="1" t="s">
+      <c r="LZ1" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="LZ1" s="1" t="s">
+      <c r="MA1" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="MA1" s="1" t="s">
+      <c r="MB1" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="MB1" s="1" t="s">
+      <c r="MC1" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="MC1" s="1" t="s">
+      <c r="MD1" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="MD1" s="1" t="s">
+      <c r="ME1" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="ME1" s="1" t="s">
+      <c r="MF1" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="MF1" s="1" t="s">
+      <c r="MG1" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="MG1" s="1" t="s">
+      <c r="MH1" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="MH1" s="1" t="s">
+      <c r="MI1" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="MI1" s="1" t="s">
+      <c r="MJ1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="MJ1" s="1" t="s">
+      <c r="MK1" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="MK1" s="1" t="s">
+      <c r="ML1" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="ML1" s="1" t="s">
+      <c r="MM1" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="MM1" s="1" t="s">
+      <c r="MN1" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="MN1" s="1" t="s">
+      <c r="MO1" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="MO1" s="1" t="s">
+      <c r="MP1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="MP1" s="1" t="s">
+      <c r="MQ1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="MQ1" s="1" t="s">
+      <c r="MR1" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="MR1" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:356" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>883</v>
-      </c>
-      <c r="I2" s="1">
-        <v>32.4</v>
-      </c>
-      <c r="J2" s="1">
-        <v>-13.8</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1">
-        <v>2.08</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="N2" s="1">
-        <v>-0.02</v>
-      </c>
-      <c r="O2" s="1">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="R2" s="1">
-        <v>-0.09</v>
-      </c>
-      <c r="S2" s="1">
-        <v>0</v>
-      </c>
-      <c r="X2" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>-0.22</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="AP2" s="1">
-        <v>155.86821</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="AR2" s="1">
-        <v>-0.90224400000000005</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>72.209999999999994</v>
-      </c>
-      <c r="AT2" s="1">
-        <v>0.68</v>
-      </c>
-      <c r="AU2" s="1">
-        <v>-0.68</v>
-      </c>
-      <c r="AV2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW2" s="1">
-        <v>6.4409999999999998</v>
-      </c>
-      <c r="AX2" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="AY2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="BA2" s="1">
-        <v>6.1980000000000004</v>
-      </c>
-      <c r="BC2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD2" s="1">
-        <v>5098</v>
-      </c>
-      <c r="BE2" s="1">
-        <v>44</v>
-      </c>
-      <c r="BF2" s="1">
-        <v>-44</v>
-      </c>
-      <c r="BG2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH2" s="1">
-        <v>1.54</v>
-      </c>
-      <c r="BI2" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="BJ2" s="1">
-        <v>-0.08</v>
-      </c>
-      <c r="BK2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BL2" s="1">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="BM2" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="BN2" s="1">
-        <v>-0.08</v>
-      </c>
-      <c r="BO2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP2" s="2">
-        <v>41773</v>
-      </c>
-      <c r="BQ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BR2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BS2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BT2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BU2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BV2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BW2" s="3">
-        <v>28.8</v>
-      </c>
-      <c r="BX2" s="3">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="BY2" s="3">
-        <v>-0.55000000000000004</v>
-      </c>
-      <c r="BZ2" s="1">
-        <v>2454930</v>
-      </c>
-      <c r="CA2" s="1">
-        <v>209.9</v>
-      </c>
-      <c r="CB2" s="1">
-        <v>-96.5</v>
-      </c>
-      <c r="CC2" s="1">
-        <v>0</v>
-      </c>
-      <c r="CD2" s="1">
-        <v>220.5</v>
-      </c>
-      <c r="CE2" s="1">
-        <v>182.2</v>
-      </c>
-      <c r="CF2" s="1">
-        <v>-320.89999999999998</v>
-      </c>
-      <c r="CG2" s="1">
-        <v>0</v>
-      </c>
-      <c r="CH2" s="1">
-        <v>14.5</v>
-      </c>
-      <c r="CI2" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="CJ2" s="1">
-        <v>-3.6</v>
-      </c>
-      <c r="CK2" s="1">
-        <v>0</v>
-      </c>
-      <c r="CX2" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="CY2" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="CZ2" s="1">
-        <v>-0.22</v>
-      </c>
-      <c r="DA2" s="1">
-        <v>0</v>
-      </c>
-      <c r="DF2" s="1">
-        <v>273.32</v>
-      </c>
-      <c r="DG2" s="1">
-        <v>111.24</v>
-      </c>
-      <c r="DH2" s="1">
-        <v>-69.92</v>
-      </c>
-      <c r="DI2" s="1">
-        <v>0</v>
-      </c>
-      <c r="DJ2" s="1">
-        <v>273.32</v>
-      </c>
-      <c r="DK2" s="1">
-        <v>111.24</v>
-      </c>
-      <c r="DL2" s="1">
-        <v>-69.92</v>
-      </c>
-      <c r="DM2" s="1">
-        <v>0</v>
-      </c>
-      <c r="EY2" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="EZ2" s="1">
-        <v>2010</v>
-      </c>
-      <c r="FA2" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="FB2" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="FC2" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="FD2" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="FE2" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="FF2" s="1">
-        <v>3</v>
-      </c>
-      <c r="FG2" s="1">
-        <v>0</v>
-      </c>
-      <c r="FH2" s="1">
-        <v>21</v>
-      </c>
-      <c r="FI2" s="1">
-        <v>17</v>
-      </c>
-      <c r="FJ2" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="FK2" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="FL2" s="4">
-        <v>40544</v>
-      </c>
-      <c r="FM2" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="FN2" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="FO2" s="1">
-        <v>10.391213990000001</v>
-      </c>
-      <c r="FP2" s="1">
-        <v>245.085309</v>
-      </c>
-      <c r="FQ2" s="1">
-        <v>44.715733999999998</v>
-      </c>
-      <c r="FR2" s="1">
-        <v>157.99359000000001</v>
-      </c>
-      <c r="FS2" s="1">
-        <v>-10.198148</v>
-      </c>
-      <c r="FT2" s="1">
-        <v>13.85</v>
-      </c>
-      <c r="FU2" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="FV2" s="1">
-        <v>-0.13</v>
-      </c>
-      <c r="FW2" s="1">
-        <v>0</v>
-      </c>
-      <c r="FX2" s="1">
-        <v>13.85</v>
-      </c>
-      <c r="FY2" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="FZ2" s="1">
-        <v>-0.13</v>
-      </c>
-      <c r="GA2" s="1">
-        <v>0</v>
-      </c>
-      <c r="GB2" s="1">
-        <v>72.209999999999994</v>
-      </c>
-      <c r="GC2" s="1">
-        <v>0.68</v>
-      </c>
-      <c r="GD2" s="1">
-        <v>-0.68</v>
-      </c>
-      <c r="GE2" s="1">
-        <v>0</v>
-      </c>
-      <c r="GF2" s="1">
-        <v>65.2</v>
-      </c>
-      <c r="GG2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="GH2" s="1">
-        <v>0</v>
-      </c>
-      <c r="GI2" s="1">
-        <v>-36.299999999999997</v>
-      </c>
-      <c r="GJ2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="GK2" s="1">
-        <v>0</v>
-      </c>
-      <c r="GL2" s="1">
-        <v>74.599999999999994</v>
-      </c>
-      <c r="GM2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="GN2" s="1">
-        <v>0</v>
-      </c>
-      <c r="GO2" s="1">
-        <v>65.2</v>
-      </c>
-      <c r="GP2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="GQ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="GR2" s="1">
-        <v>-36.299999999999997</v>
-      </c>
-      <c r="GS2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="GT2" s="1">
-        <v>0</v>
-      </c>
-      <c r="GU2" s="1">
-        <v>74.599999999999994</v>
-      </c>
-      <c r="GV2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="GW2" s="1">
-        <v>0</v>
-      </c>
-      <c r="GX2" s="1">
-        <v>7.29</v>
-      </c>
-      <c r="GY2" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="GZ2" s="1">
-        <v>-0.18</v>
-      </c>
-      <c r="HA2" s="1">
-        <v>0</v>
-      </c>
-      <c r="HB2" s="1">
-        <v>5</v>
-      </c>
-      <c r="HC2" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="HE2" s="1">
-        <v>0</v>
-      </c>
-      <c r="HF2" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="HG2" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="HH2" s="1">
-        <v>-0.1</v>
-      </c>
-      <c r="HI2" s="1">
-        <v>0</v>
-      </c>
-      <c r="HJ2" s="1">
-        <v>1.1639999999999999</v>
-      </c>
-      <c r="HK2" s="1">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="HL2" s="1">
-        <v>-3.0000000000000001E-3</v>
-      </c>
-      <c r="HM2" s="1">
-        <v>0</v>
-      </c>
-      <c r="HR2" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="HS2" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="HT2" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="HU2" s="1">
-        <v>0</v>
-      </c>
-      <c r="HV2" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="HW2" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="HX2" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="HY2" s="1">
-        <v>-0.4</v>
-      </c>
-      <c r="IA2" s="1">
-        <v>2.77</v>
-      </c>
-      <c r="IB2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="IC2" s="1">
-        <v>-0.5</v>
-      </c>
-      <c r="ID2" s="1">
-        <v>0</v>
-      </c>
-      <c r="IO2" s="1">
-        <v>3</v>
-      </c>
-      <c r="IP2" s="1">
-        <v>0</v>
-      </c>
-      <c r="IQ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="IR2" s="1">
-        <v>2</v>
-      </c>
-      <c r="IS2" s="1">
-        <v>0</v>
-      </c>
-      <c r="IT2" s="1">
-        <v>3</v>
-      </c>
-      <c r="IU2" s="1">
-        <v>1</v>
-      </c>
-      <c r="IY2" s="1">
-        <v>6.4409999999999998</v>
-      </c>
-      <c r="IZ2" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="JA2" s="1">
-        <v>0</v>
-      </c>
-      <c r="JB2" s="1">
-        <v>7.399</v>
-      </c>
-      <c r="JC2" s="1">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="JD2" s="1">
-        <v>0</v>
-      </c>
-      <c r="JK2" s="1">
-        <v>5.2919999999999998</v>
-      </c>
-      <c r="JL2" s="1">
-        <v>0.33800000000000002</v>
-      </c>
-      <c r="JM2" s="1">
-        <v>0</v>
-      </c>
-      <c r="JN2" s="1">
-        <v>4.4859999999999998</v>
-      </c>
-      <c r="JO2" s="1">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="JP2" s="1">
-        <v>0</v>
-      </c>
-      <c r="JQ2" s="1">
-        <v>4.2850000000000001</v>
-      </c>
-      <c r="JR2" s="1">
-        <v>1.6E-2</v>
-      </c>
-      <c r="JS2" s="1">
-        <v>0</v>
-      </c>
-      <c r="JT2" s="1">
-        <v>4.0940000000000003</v>
-      </c>
-      <c r="JU2" s="1">
-        <v>0.32700000000000001</v>
-      </c>
-      <c r="JV2" s="1">
-        <v>0</v>
-      </c>
-      <c r="JW2" s="1">
-        <v>3.5979999999999999</v>
-      </c>
-      <c r="JX2" s="1">
-        <v>0.156</v>
-      </c>
-      <c r="JY2" s="1">
-        <v>0</v>
-      </c>
-      <c r="JZ2" s="1">
-        <v>4.2539999999999996</v>
-      </c>
-      <c r="KA2" s="1">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="KB2" s="1">
-        <v>0</v>
-      </c>
-      <c r="KC2" s="1">
-        <v>4.2009999999999996</v>
-      </c>
-      <c r="KD2" s="1">
-        <v>2.4E-2</v>
-      </c>
-      <c r="KE2" s="1">
-        <v>0</v>
-      </c>
-      <c r="LA2" s="3">
-        <v>3.8</v>
-      </c>
-      <c r="LB2" s="3">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="LC2" s="1">
-        <v>0</v>
-      </c>
-      <c r="LD2" s="3">
-        <v>2.56</v>
-      </c>
-      <c r="LF2" s="1">
-        <v>1</v>
-      </c>
-      <c r="LG2" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="LI2" s="1">
-        <v>1</v>
-      </c>
-      <c r="LJ2" s="3">
-        <v>-0.91600000000000004</v>
-      </c>
-      <c r="LL2" s="1">
-        <v>1</v>
-      </c>
-      <c r="LM2" s="1">
-        <v>17</v>
-      </c>
-      <c r="LQ2" s="1">
-        <v>0.95799999999999996</v>
-      </c>
-      <c r="LR2" s="1">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="LS2" s="1">
-        <v>0</v>
-      </c>
-      <c r="LZ2" s="1">
-        <v>0.80600000000000005</v>
-      </c>
-      <c r="MA2" s="1">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="MB2" s="1">
-        <v>0</v>
-      </c>
-      <c r="MC2" s="1">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="MD2" s="1">
-        <v>7.8E-2</v>
-      </c>
-      <c r="ME2" s="1">
-        <v>0</v>
-      </c>
-      <c r="MF2" s="1">
-        <v>1.0069999999999999</v>
-      </c>
-      <c r="MG2" s="1">
-        <v>0.33800000000000002</v>
-      </c>
-      <c r="MH2" s="1">
-        <v>0</v>
-      </c>
-      <c r="MI2" s="1">
-        <v>0.57199999999999995</v>
-      </c>
-      <c r="MJ2" s="1">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="MK2" s="1">
-        <v>0</v>
-      </c>
-      <c r="ML2" s="1">
-        <v>0.34200000000000003</v>
-      </c>
-      <c r="MM2" s="1">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="MN2" s="1">
-        <v>0</v>
-      </c>
-      <c r="MO2" s="1">
-        <v>0.42699999999999999</v>
-      </c>
-      <c r="MP2" s="1">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="MQ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="MR2" s="1">
-        <v>8</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="BP2" s="2"/>
+      <c r="BW2" s="3"/>
+      <c r="BX2" s="3"/>
+      <c r="BY2" s="3"/>
+      <c r="FL2" s="4"/>
+      <c r="LA2" s="3"/>
+      <c r="LB2" s="3"/>
+      <c r="LD2" s="3"/>
+      <c r="LG2" s="3"/>
+      <c r="LJ2" s="3"/>
     </row>
     <row r="3" spans="1:356" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1">
-        <v>52</v>
-      </c>
-      <c r="M3" s="1">
-        <v>6</v>
-      </c>
-      <c r="N3" s="1">
-        <v>-6</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="X3" s="1">
-        <v>24.5</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>-2.5</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="AK3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="AP3" s="1">
-        <v>20.712243000000001</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="AR3" s="1">
-        <v>-24.664048999999999</v>
-      </c>
-      <c r="AS3" s="1">
-        <v>36</v>
-      </c>
-      <c r="AT3" s="1">
-        <v>4</v>
-      </c>
-      <c r="AU3" s="1">
-        <v>-4</v>
-      </c>
-      <c r="AV3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="1">
-        <v>14.24</v>
-      </c>
-      <c r="AX3" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AY3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AZ3" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="BA3" s="1">
-        <v>12.903</v>
-      </c>
-      <c r="BC3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD3" s="1">
-        <v>3530</v>
-      </c>
-      <c r="BE3" s="1">
-        <v>50</v>
-      </c>
-      <c r="BF3" s="1">
-        <v>-50</v>
-      </c>
-      <c r="BG3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH3" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="BI3" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="BJ3" s="1">
-        <v>-0.05</v>
-      </c>
-      <c r="BK3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP3" s="2">
-        <v>41773</v>
-      </c>
-      <c r="BQ3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BR3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BS3" s="1">
-        <v>1</v>
-      </c>
-      <c r="BT3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BU3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BV3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BW3" s="3">
-        <v>1440</v>
-      </c>
-      <c r="BX3" s="3">
-        <v>231</v>
-      </c>
-      <c r="BY3" s="3">
-        <v>-231</v>
-      </c>
-      <c r="CT3" s="1">
-        <v>24.5</v>
-      </c>
-      <c r="CU3" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="CV3" s="1">
-        <v>-2.5</v>
-      </c>
-      <c r="CW3" s="1">
-        <v>0</v>
-      </c>
-      <c r="DB3" s="1">
-        <v>7786.5</v>
-      </c>
-      <c r="DC3" s="1">
-        <v>794.5</v>
-      </c>
-      <c r="DD3" s="1">
-        <v>-794.5</v>
-      </c>
-      <c r="DE3" s="1">
-        <v>0</v>
-      </c>
-      <c r="DJ3" s="1">
-        <v>7786.5</v>
-      </c>
-      <c r="DK3" s="1">
-        <v>794.5</v>
-      </c>
-      <c r="DL3" s="1">
-        <v>-794.5</v>
-      </c>
-      <c r="DM3" s="1">
-        <v>0</v>
-      </c>
-      <c r="EY3" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="EZ3" s="1">
-        <v>2013</v>
-      </c>
-      <c r="FA3" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="FB3" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="FC3" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD3" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="FE3" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="FF3" s="1">
-        <v>3</v>
-      </c>
-      <c r="FG3" s="1">
-        <v>0</v>
-      </c>
-      <c r="FH3" s="1">
-        <v>9</v>
-      </c>
-      <c r="FI3" s="1">
-        <v>6</v>
-      </c>
-      <c r="FJ3" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="FL3" s="4">
-        <v>41487</v>
-      </c>
-      <c r="FO3" s="1">
-        <v>1.3808161999999999</v>
-      </c>
-      <c r="FP3" s="1">
-        <v>195.448768</v>
-      </c>
-      <c r="FQ3" s="1">
-        <v>-82.520165000000006</v>
-      </c>
-      <c r="FR3" s="1">
-        <v>8.6224129999999999</v>
-      </c>
-      <c r="FS3" s="1">
-        <v>-30.711243</v>
-      </c>
-      <c r="FW3" s="1">
-        <v>0</v>
-      </c>
-      <c r="FX3" s="1">
-        <v>29.53</v>
-      </c>
-      <c r="FY3" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="FZ3" s="1">
-        <v>-7.0000000000000007E-2</v>
-      </c>
-      <c r="GA3" s="1">
-        <v>0</v>
-      </c>
-      <c r="GB3" s="1">
-        <v>33.86</v>
-      </c>
-      <c r="GC3" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="GD3" s="1">
-        <v>-0.09</v>
-      </c>
-      <c r="GE3" s="1">
-        <v>0</v>
-      </c>
-      <c r="GF3" s="1">
-        <v>120.5</v>
-      </c>
-      <c r="GG3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="GH3" s="1">
-        <v>0</v>
-      </c>
-      <c r="GI3" s="1">
-        <v>-123.4</v>
-      </c>
-      <c r="GJ3" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="GK3" s="1">
-        <v>0</v>
-      </c>
-      <c r="GL3" s="1">
-        <v>172.4</v>
-      </c>
-      <c r="GM3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="GN3" s="1">
-        <v>0</v>
-      </c>
-      <c r="GO3" s="1">
-        <v>120.5</v>
-      </c>
-      <c r="GP3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="GQ3" s="1">
-        <v>0</v>
-      </c>
-      <c r="GR3" s="1">
-        <v>-123.4</v>
-      </c>
-      <c r="GS3" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="GT3" s="1">
-        <v>0</v>
-      </c>
-      <c r="GU3" s="1">
-        <v>172.4</v>
-      </c>
-      <c r="GV3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="GW3" s="1">
-        <v>0</v>
-      </c>
-      <c r="GX3" s="1">
-        <v>9.6</v>
-      </c>
-      <c r="GY3" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="GZ3" s="1">
-        <v>-0.7</v>
-      </c>
-      <c r="HA3" s="1">
-        <v>0</v>
-      </c>
-      <c r="HB3" s="1">
-        <v>6.35</v>
-      </c>
-      <c r="HC3" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="HE3" s="1">
-        <v>0</v>
-      </c>
-      <c r="HJ3" s="1">
-        <v>-1.72</v>
-      </c>
-      <c r="HK3" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="HL3" s="1">
-        <v>-0.11</v>
-      </c>
-      <c r="HM3" s="1">
-        <v>0</v>
-      </c>
-      <c r="HW3" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="HX3" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="HY3" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="IO3" s="1">
-        <v>0</v>
-      </c>
-      <c r="IP3" s="1">
-        <v>0</v>
-      </c>
-      <c r="IQ3" s="1">
-        <v>0</v>
-      </c>
-      <c r="IR3" s="1">
-        <v>0</v>
-      </c>
-      <c r="IS3" s="1">
-        <v>0</v>
-      </c>
-      <c r="IT3" s="1">
-        <v>3</v>
-      </c>
-      <c r="IU3" s="1">
-        <v>0</v>
-      </c>
-      <c r="IY3" s="1">
-        <v>14.24</v>
-      </c>
-      <c r="IZ3" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="JA3" s="1">
-        <v>0</v>
-      </c>
-      <c r="JK3" s="1">
-        <v>10.084</v>
-      </c>
-      <c r="JL3" s="1">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="JM3" s="1">
-        <v>0</v>
-      </c>
-      <c r="JN3" s="1">
-        <v>9.4700000000000006</v>
-      </c>
-      <c r="JO3" s="1">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="JP3" s="1">
-        <v>0</v>
-      </c>
-      <c r="JQ3" s="1">
-        <v>9.1980000000000004</v>
-      </c>
-      <c r="JR3" s="1">
-        <v>2.4E-2</v>
-      </c>
-      <c r="JS3" s="1">
-        <v>0</v>
-      </c>
-      <c r="JT3" s="1">
-        <v>9.0220000000000002</v>
-      </c>
-      <c r="JU3" s="1">
-        <v>2.3E-2</v>
-      </c>
-      <c r="JV3" s="1">
-        <v>0</v>
-      </c>
-      <c r="JW3" s="1">
-        <v>8.8569999999999993</v>
-      </c>
-      <c r="JX3" s="1">
-        <v>1.9E-2</v>
-      </c>
-      <c r="JY3" s="1">
-        <v>0</v>
-      </c>
-      <c r="JZ3" s="1">
-        <v>8.7469999999999999</v>
-      </c>
-      <c r="KA3" s="1">
-        <v>3.1E-2</v>
-      </c>
-      <c r="KB3" s="1">
-        <v>0</v>
-      </c>
-      <c r="KC3" s="1">
-        <v>8.298</v>
-      </c>
-      <c r="KD3" s="1">
-        <v>0.317</v>
-      </c>
-      <c r="KE3" s="1">
-        <v>0</v>
-      </c>
-      <c r="LM3" s="1">
-        <v>9</v>
-      </c>
-      <c r="LZ3" s="1">
-        <v>0.61399999999999999</v>
-      </c>
-      <c r="MA3" s="1">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="MB3" s="1">
-        <v>0</v>
-      </c>
-      <c r="MC3" s="1">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="MD3" s="1">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="ME3" s="1">
-        <v>0</v>
-      </c>
-      <c r="MF3" s="1">
-        <v>0.88600000000000001</v>
-      </c>
-      <c r="MG3" s="1">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="MH3" s="1">
-        <v>0</v>
-      </c>
-      <c r="MR3" s="1">
-        <v>3</v>
-      </c>
+      <c r="BP3" s="2"/>
+      <c r="BW3" s="3"/>
+      <c r="BX3" s="3"/>
+      <c r="BY3" s="3"/>
+      <c r="FL3" s="4"/>
     </row>
     <row r="4" spans="1:356" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BP4" s="2"/>

</xml_diff>